<commit_message>
Update Pizza Shop Project
</commit_message>
<xml_diff>
--- a/Prompts/Matrices/Pizza Shop IVR.xlsx
+++ b/Prompts/Matrices/Pizza Shop IVR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IST\Moaz\Work\Training\internship-material\Prompts\Matrices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE457F8-9C94-44E5-8C8D-545B1AFC29B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8859F7-372C-4E97-9078-B493B949A853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Filename</t>
   </si>
@@ -43,12 +43,6 @@
     <t>MainMenu.wav</t>
   </si>
   <si>
-    <t>Order pizza, press 1. Track your order, press 2. Speak to staff, press 3.</t>
-  </si>
-  <si>
-    <t>لطلب بيتزا، اضغط 1. لتتبع طلبك، اضغط 2. للتحدث مع الموظفين، اضغط 3.</t>
-  </si>
-  <si>
     <t>NoInput.wav</t>
   </si>
   <si>
@@ -110,6 +104,21 @@
   </si>
   <si>
     <t>شكراً لاتصالك ببيتزا توني!</t>
+  </si>
+  <si>
+    <t>EnterOrderNumber.wav</t>
+  </si>
+  <si>
+    <t>Please enter your 4-digit order number.</t>
+  </si>
+  <si>
+    <t>يرجى إدخال رقم طلبك المكون من 4 أرقام.</t>
+  </si>
+  <si>
+    <t>To Speak to an agent, press 1. To Order pizza, press 2. To Track your order, press 3.</t>
+  </si>
+  <si>
+    <t>للتحدث مع أحد موظفي خدمة العملاء، اضغط 1. لطلب بيتزا، اضغط 2. لتتبع طلبك، اضغط 3.</t>
   </si>
 </sst>
 </file>
@@ -165,8 +174,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D9226770-06A5-4883-AAF5-43DDB9FB33B8}" name="Table1" displayName="Table1" ref="A1:C10" totalsRowShown="0">
-  <autoFilter ref="A1:C10" xr:uid="{D9226770-06A5-4883-AAF5-43DDB9FB33B8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D9226770-06A5-4883-AAF5-43DDB9FB33B8}" name="Table1" displayName="Table1" ref="A1:C11" totalsRowShown="0">
+  <autoFilter ref="A1:C11" xr:uid="{D9226770-06A5-4883-AAF5-43DDB9FB33B8}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{431E7D01-4C8C-45A7-9890-7F9DAB5E3FF8}" name="Filename"/>
     <tableColumn id="2" xr3:uid="{6A61AEBB-1DDD-4534-B106-0317F365822A}" name="English Prompt"/>
@@ -498,20 +507,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -522,7 +531,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -533,98 +542,110 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C10" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>25</v>
       </c>
-      <c r="C9" t="s">
+      <c r="B11" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C11" t="s">
         <v>27</v>
-      </c>
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>